<commit_message>
Some Start Notebooks are improved
</commit_message>
<xml_diff>
--- a/Case_studies/Montefrio/soil/K_factor.xlsx
+++ b/Case_studies/Montefrio/soil/K_factor.xlsx
@@ -468,7 +468,7 @@
         <v>4132795.83</v>
       </c>
       <c r="D2" t="n">
-        <v>0.03027679616883376</v>
+        <v>0.03080416072544545</v>
       </c>
     </row>
     <row r="3">
@@ -484,7 +484,7 @@
         <v>4132795.52</v>
       </c>
       <c r="D3" t="n">
-        <v>0.03211196723988209</v>
+        <v>0.03291997439496604</v>
       </c>
     </row>
     <row r="4">
@@ -500,7 +500,7 @@
         <v>4132693.41999999</v>
       </c>
       <c r="D4" t="n">
-        <v>0.03118066565640312</v>
+        <v>0.03173670924868253</v>
       </c>
     </row>
     <row r="5">
@@ -516,7 +516,7 @@
         <v>4132701.14999999</v>
       </c>
       <c r="D5" t="n">
-        <v>0.03255124508747329</v>
+        <v>0.03276935887518878</v>
       </c>
     </row>
     <row r="6">
@@ -532,7 +532,7 @@
         <v>4132695.39</v>
       </c>
       <c r="D6" t="n">
-        <v>0.02817641991613139</v>
+        <v>0.0283269227693807</v>
       </c>
     </row>
     <row r="7">
@@ -548,7 +548,7 @@
         <v>4132596.54999999</v>
       </c>
       <c r="D7" t="n">
-        <v>0.0290029518881147</v>
+        <v>0.02940634096020636</v>
       </c>
     </row>
     <row r="8">
@@ -564,7 +564,7 @@
         <v>4132596.39999999</v>
       </c>
       <c r="D8" t="n">
-        <v>0.03087205139797026</v>
+        <v>0.03113203610901872</v>
       </c>
     </row>
     <row r="9">
@@ -580,7 +580,7 @@
         <v>4132599.48</v>
       </c>
       <c r="D9" t="n">
-        <v>0.03010465843129768</v>
+        <v>0.03101677899956277</v>
       </c>
     </row>
     <row r="10">
@@ -596,7 +596,7 @@
         <v>4132497.47999999</v>
       </c>
       <c r="D10" t="n">
-        <v>0.0314902006265529</v>
+        <v>0.03230892957494577</v>
       </c>
     </row>
     <row r="11">
@@ -612,7 +612,7 @@
         <v>4132486.27</v>
       </c>
       <c r="D11" t="n">
-        <v>0.02982798181004403</v>
+        <v>0.03011790861975424</v>
       </c>
     </row>
     <row r="12">
@@ -628,7 +628,7 @@
         <v>4132696.45</v>
       </c>
       <c r="D12" t="n">
-        <v>0.02780351162448026</v>
+        <v>0.02815258978502906</v>
       </c>
     </row>
     <row r="13">
@@ -644,7 +644,7 @@
         <v>4132694.79</v>
       </c>
       <c r="D13" t="n">
-        <v>0.02780351162448026</v>
+        <v>0.02819516029241307</v>
       </c>
     </row>
     <row r="14">
@@ -660,7 +660,7 @@
         <v>4132645.39999999</v>
       </c>
       <c r="D14" t="n">
-        <v>0.02598549206117898</v>
+        <v>0.02593060120982496</v>
       </c>
     </row>
     <row r="15">
@@ -676,7 +676,7 @@
         <v>4132600.49</v>
       </c>
       <c r="D15" t="n">
-        <v>0.02717376285790288</v>
+        <v>0.0268958067669696</v>
       </c>
     </row>
     <row r="16">
@@ -692,7 +692,7 @@
         <v>4132693.35</v>
       </c>
       <c r="D16" t="n">
-        <v>0.02780351162448026</v>
+        <v>0.02812704748059866</v>
       </c>
     </row>
     <row r="17">
@@ -708,7 +708,7 @@
         <v>4132648.50999999</v>
       </c>
       <c r="D17" t="n">
-        <v>0.02666843825930344</v>
+        <v>0.02684052924108888</v>
       </c>
     </row>
     <row r="18">
@@ -724,7 +724,7 @@
         <v>4132597.30599999</v>
       </c>
       <c r="D18" t="n">
-        <v>0.02643998540370356</v>
+        <v>0.02650545619337022</v>
       </c>
     </row>
     <row r="19">
@@ -740,7 +740,7 @@
         <v>4132548.68</v>
       </c>
       <c r="D19" t="n">
-        <v>0.02767341971026861</v>
+        <v>0.02790010728497521</v>
       </c>
     </row>
     <row r="20">
@@ -756,7 +756,7 @@
         <v>4132494.2</v>
       </c>
       <c r="D20" t="n">
-        <v>0.02585882555296094</v>
+        <v>0.02597351103877943</v>
       </c>
     </row>
     <row r="21">
@@ -772,7 +772,7 @@
         <v>4132497.17</v>
       </c>
       <c r="D21" t="n">
-        <v>0.0290029518881147</v>
+        <v>0.0296944760117004</v>
       </c>
     </row>
     <row r="22">
@@ -788,7 +788,7 @@
         <v>4132399.77</v>
       </c>
       <c r="D22" t="n">
-        <v>0.02704478527552455</v>
+        <v>0.0270604339760255</v>
       </c>
     </row>
     <row r="23">
@@ -804,7 +804,7 @@
         <v>4132446.52999999</v>
       </c>
       <c r="D23" t="n">
-        <v>0.0248908614256244</v>
+        <v>0.02494365756456133</v>
       </c>
     </row>
     <row r="24">
@@ -820,7 +820,7 @@
         <v>4132544.74</v>
       </c>
       <c r="D24" t="n">
-        <v>0.02858865253495291</v>
+        <v>0.02873629839000677</v>
       </c>
     </row>
     <row r="25">
@@ -836,7 +836,7 @@
         <v>4132498.29</v>
       </c>
       <c r="D25" t="n">
-        <v>0.02868263227117995</v>
+        <v>0.02881301850008587</v>
       </c>
     </row>
     <row r="26">
@@ -852,7 +852,7 @@
         <v>4132441.08</v>
       </c>
       <c r="D26" t="n">
-        <v>0.0314902006265529</v>
+        <v>0.03252251103974391</v>
       </c>
     </row>
     <row r="27">
@@ -868,7 +868,7 @@
         <v>4132403.66</v>
       </c>
       <c r="D27" t="n">
-        <v>0.0314902006265529</v>
+        <v>0.03215467629481378</v>
       </c>
     </row>
     <row r="28">
@@ -884,7 +884,7 @@
         <v>4132407.09</v>
       </c>
       <c r="D28" t="n">
-        <v>0.03056437504106823</v>
+        <v>0.03098328617885059</v>
       </c>
     </row>
     <row r="29">
@@ -900,7 +900,7 @@
         <v>4132399.41999999</v>
       </c>
       <c r="D29" t="n">
-        <v>0.03043006610755779</v>
+        <v>0.03099696377809688</v>
       </c>
     </row>
     <row r="30">
@@ -916,7 +916,7 @@
         <v>4132360.22999999</v>
       </c>
       <c r="D30" t="n">
-        <v>0.02805502893645768</v>
+        <v>0.02832605429739422</v>
       </c>
     </row>
   </sheetData>

</xml_diff>